<commit_message>
PDF generating code added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Comparison</t>
+          <t>Above / Below</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -476,1022 +476,1262 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>150</v>
-      </c>
-      <c r="C2" t="n">
-        <v>7654</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3902</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>7654</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3902</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>160</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4567</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2363.5</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4567</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2363.5</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>170</v>
-      </c>
-      <c r="C4" t="n">
-        <v>9876</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5023</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9876</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5023</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>180</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5432</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2806</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5432</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2806</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>190</v>
-      </c>
-      <c r="C6" t="n">
-        <v>6543</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3366.5</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>6543</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>3366.5</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>200</v>
-      </c>
-      <c r="C7" t="n">
-        <v>8764</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4482</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8764</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4482</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>210</v>
-      </c>
-      <c r="C8" t="n">
-        <v>9876</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5043</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9876</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>5043</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>220</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3456</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1838</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>220</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1838</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>230</v>
-      </c>
-      <c r="C10" t="n">
-        <v>6545</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3387.5</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>6545</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3387.5</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>240</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1234</v>
-      </c>
-      <c r="D11" t="n">
-        <v>737</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>737</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>250</v>
-      </c>
-      <c r="C12" t="n">
-        <v>6432</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3341</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>6432</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3341</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>260</v>
-      </c>
-      <c r="C13" t="n">
-        <v>9786</v>
-      </c>
-      <c r="D13" t="n">
-        <v>5023</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>260</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9786</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>5023</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>270</v>
-      </c>
-      <c r="C14" t="n">
-        <v>8977</v>
-      </c>
-      <c r="D14" t="n">
-        <v>4623.5</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>270</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>8977</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4623.5</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>280</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3456</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1868</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>280</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3456</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1868</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>290</v>
-      </c>
-      <c r="C16" t="n">
-        <v>7866</v>
-      </c>
-      <c r="D16" t="n">
-        <v>4078</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>7866</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4078</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>300</v>
-      </c>
-      <c r="C17" t="n">
-        <v>5353</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2826.5</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>5353</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2826.5</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>310</v>
-      </c>
-      <c r="C18" t="n">
-        <v>7564</v>
-      </c>
-      <c r="D18" t="n">
-        <v>3937</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>310</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>7564</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>3937</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>320</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4738</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2529</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4738</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2529</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>330</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2468</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1399</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2468</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1399</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>340</v>
-      </c>
-      <c r="C21" t="n">
-        <v>8346</v>
-      </c>
-      <c r="D21" t="n">
-        <v>4343</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>8346</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>4343</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="n">
-        <v>341</v>
-      </c>
-      <c r="C22" t="n">
-        <v>8347</v>
-      </c>
-      <c r="D22" t="n">
-        <v>4344</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8347</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>4344</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="n">
-        <v>342</v>
-      </c>
-      <c r="C23" t="n">
-        <v>8348</v>
-      </c>
-      <c r="D23" t="n">
-        <v>4345</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>342</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>8348</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>4345</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="n">
-        <v>343</v>
-      </c>
-      <c r="C24" t="n">
-        <v>8349</v>
-      </c>
-      <c r="D24" t="n">
-        <v>4346</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>343</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>8349</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>4346</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="n">
-        <v>344</v>
-      </c>
-      <c r="C25" t="n">
-        <v>8350</v>
-      </c>
-      <c r="D25" t="n">
-        <v>4347</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>8350</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>4347</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="n">
-        <v>345</v>
-      </c>
-      <c r="C26" t="n">
-        <v>8351</v>
-      </c>
-      <c r="D26" t="n">
-        <v>4348</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>8351</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>4348</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="n">
-        <v>346</v>
-      </c>
-      <c r="C27" t="n">
-        <v>8352</v>
-      </c>
-      <c r="D27" t="n">
-        <v>4349</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>8352</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>4349</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="n">
-        <v>347</v>
-      </c>
-      <c r="C28" t="n">
-        <v>8353</v>
-      </c>
-      <c r="D28" t="n">
-        <v>4350</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>8353</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>4350</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="n">
-        <v>348</v>
-      </c>
-      <c r="C29" t="n">
-        <v>8354</v>
-      </c>
-      <c r="D29" t="n">
-        <v>4351</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>348</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>8354</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>4351</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="n">
-        <v>349</v>
-      </c>
-      <c r="C30" t="n">
-        <v>8355</v>
-      </c>
-      <c r="D30" t="n">
-        <v>4352</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>349</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>8355</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>4352</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" t="n">
-        <v>350</v>
-      </c>
-      <c r="C31" t="n">
-        <v>8356</v>
-      </c>
-      <c r="D31" t="n">
-        <v>4353</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>8356</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>4353</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Above</t>
+          <t>Below</t>
         </is>
       </c>
     </row>

</xml_diff>